<commit_message>
add work time log to Time Allocation.xlsx
</commit_message>
<xml_diff>
--- a/Time Allocation.xlsx
+++ b/Time Allocation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t xml:space="preserve">i. Unit test cases planning </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +72,62 @@
   </si>
   <si>
     <t>3/23 03:10 P.M.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20 min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20 min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/26 07:30 P.M.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/26 07:40 P.M.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/26 08:40 P.M.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60 min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/26 07:10 P.M.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/26 07:00 P.M.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50 min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30 min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/27 02:20 P.M.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/27 03:10 P.M.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/27 04:00 P.M.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/27 03:30 P.M.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -474,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -516,6 +572,17 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="9" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>4</v>
@@ -545,6 +612,17 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="17" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>5</v>
@@ -575,6 +653,39 @@
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
@@ -656,6 +767,17 @@
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
     </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>